<commit_message>
exploration of data and consideration on tests to perform in R comments
</commit_message>
<xml_diff>
--- a/SAPS_2016_Glossary.xlsx
+++ b/SAPS_2016_Glossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davy Sheehy\Desktop\ABDAFinalAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76978A1B-E57A-4CBC-BE01-A66FF62E7141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4425802-552F-4CE0-AB77-E795590AD577}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5366,8 +5366,8 @@
   <dimension ref="A1:F800"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A621" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D644" sqref="D644"/>
+      <pane ySplit="1" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D647" sqref="D647"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>